<commit_message>
Inclusão da apresentação do dia 3/8/16
</commit_message>
<xml_diff>
--- a/EngenhariaSoftware/Regras de negócio v2.0.xlsx
+++ b/EngenhariaSoftware/Regras de negócio v2.0.xlsx
@@ -1015,8 +1015,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Revisão das regras de negócio
</commit_message>
<xml_diff>
--- a/EngenhariaSoftware/Regras de negócio v2.0.xlsx
+++ b/EngenhariaSoftware/Regras de negócio v2.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
   <si>
     <t>Descrição</t>
   </si>
@@ -296,21 +296,12 @@
     <t>RN25</t>
   </si>
   <si>
-    <t>O cliente pode requisitar serviços ilimitadamente.</t>
-  </si>
-  <si>
     <t>RN26</t>
   </si>
   <si>
-    <t>Para o cliente requisitar um serviço é necessário estar cadastrado.</t>
-  </si>
-  <si>
     <t>RN27</t>
   </si>
   <si>
-    <t>A requisição de serviço poderá ficar aberta até 30 dias corridos.</t>
-  </si>
-  <si>
     <t>RN28</t>
   </si>
   <si>
@@ -326,15 +317,9 @@
     <t>RN30</t>
   </si>
   <si>
-    <t xml:space="preserve">O leilão deve conter data de abertura e de término, título e descrição do serviço. </t>
-  </si>
-  <si>
     <t>RN31</t>
   </si>
   <si>
-    <t xml:space="preserve">O lance do autônomo deve conter valor e uma descrição de proposta. </t>
-  </si>
-  <si>
     <t>RN32</t>
   </si>
   <si>
@@ -344,34 +329,37 @@
     <t>RN33</t>
   </si>
   <si>
-    <t>O autônomo poderá fazer pesquisa de serviços</t>
-  </si>
-  <si>
     <t>RN34</t>
   </si>
   <si>
     <t>Os lances mais novos do leilão devem ser exibidos primeiro.</t>
   </si>
   <si>
-    <t>Desde que o lance anterior tenha sido rejeitado.</t>
-  </si>
-  <si>
-    <t>não deve ter descrição.</t>
-  </si>
-  <si>
     <t>RN35</t>
   </si>
   <si>
-    <t>Um autonomo pode procurar novos leilões e visualiza-los</t>
-  </si>
-  <si>
-    <t>RN36</t>
-  </si>
-  <si>
     <t>Autonomo não pode fazer lances em areas de atuação que não sejam pertencentes a ele.</t>
   </si>
   <si>
     <t>Colunas1</t>
+  </si>
+  <si>
+    <t>O cliente pode abrir leilões ilimitadamente.</t>
+  </si>
+  <si>
+    <t>Para o cliente abrir um leilão, é necessário ser cadastrado no sistema.</t>
+  </si>
+  <si>
+    <t>O leilão poderá ficar aberto por até 30 dias.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O leilão deve conter data de abertura e de término, data de previsão, título e descrição do serviço. </t>
+  </si>
+  <si>
+    <t>Um autonomo pode procurar novos leilões e visualizá-los.</t>
+  </si>
+  <si>
+    <t>O autônomo poderá fazer pesquisa de leilões.</t>
   </si>
 </sst>
 </file>
@@ -426,7 +414,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -527,8 +515,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C37" totalsRowShown="0">
-  <autoFilter ref="A1:C37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C36" totalsRowShown="0">
+  <autoFilter ref="A1:C36"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Código" dataDxfId="0"/>
     <tableColumn id="2" name="Descrição"/>
@@ -1035,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1054,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1177,7 +1165,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>68</v>
       </c>
@@ -1185,7 +1173,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>69</v>
       </c>
@@ -1193,7 +1181,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>71</v>
       </c>
@@ -1201,7 +1189,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
@@ -1209,7 +1197,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
         <v>73</v>
       </c>
@@ -1217,7 +1205,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>74</v>
       </c>
@@ -1225,18 +1213,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
         <v>76</v>
       </c>
       <c r="B23" t="s">
         <v>85</v>
       </c>
-      <c r="C23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>78</v>
       </c>
@@ -1244,7 +1229,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>87</v>
       </c>
@@ -1252,103 +1237,92 @@
         <v>88</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>89</v>
       </c>
       <c r="B26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="B27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="B29" t="s">
         <v>93</v>
       </c>
-      <c r="B28" t="s">
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="B30" t="s">
         <v>95</v>
       </c>
-      <c r="B29" t="s">
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="B31" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="B30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="B32" t="s">
         <v>99</v>
-      </c>
-      <c r="B31" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B32" t="s">
-        <v>102</v>
-      </c>
-      <c r="C32" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B33" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B35" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="B37" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correção dos casos de uso; Finalização do documento de requisitos
</commit_message>
<xml_diff>
--- a/EngenhariaSoftware/Regras de negócio v2.0.xlsx
+++ b/EngenhariaSoftware/Regras de negócio v2.0.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
   <si>
     <t>Descrição</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>O autônomo poderá fazer pesquisa de leilões.</t>
+  </si>
+  <si>
+    <t>O autônomo poderá ou não exibir suas informações de localização.</t>
   </si>
 </sst>
 </file>
@@ -515,8 +518,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C36" totalsRowShown="0">
-  <autoFilter ref="A1:C36"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C37" totalsRowShown="0">
+  <autoFilter ref="A1:C37"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Código" dataDxfId="0"/>
     <tableColumn id="2" name="Descrição"/>
@@ -1023,15 +1026,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="101.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1323,6 +1327,12 @@
       </c>
       <c r="B36" t="s">
         <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documentos finalizados para a 1º prévia
</commit_message>
<xml_diff>
--- a/EngenhariaSoftware/Regras de negócio v2.0.xlsx
+++ b/EngenhariaSoftware/Regras de negócio v2.0.xlsx
@@ -14,7 +14,6 @@
   <sheets>
     <sheet name="Prévia 1" sheetId="1" r:id="rId1"/>
     <sheet name="Prévia2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -24,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="109">
   <si>
     <t>Descrição</t>
   </si>
@@ -176,9 +175,6 @@
     <t>RN04</t>
   </si>
   <si>
-    <t>O profissional autônomo deve se cadastrar usando e-mail para contato.</t>
-  </si>
-  <si>
     <t>RN05</t>
   </si>
   <si>
@@ -212,21 +208,12 @@
     <t>RN12</t>
   </si>
   <si>
-    <t>O sistema não interfere no método de pagamento do serviço prestado pelo trabalhador autônomo.</t>
-  </si>
-  <si>
     <t>RN13</t>
   </si>
   <si>
-    <t>O cliente precisa ter a idade mínima de 18 anos.</t>
-  </si>
-  <si>
     <t>RN14</t>
   </si>
   <si>
-    <t>O sistema de busca apresentará o resultado de acordo com a classificação do profissional autônomo no sistema.</t>
-  </si>
-  <si>
     <t>RN15</t>
   </si>
   <si>
@@ -236,9 +223,6 @@
     <t>RN17</t>
   </si>
   <si>
-    <t>O sistema permite que o autônomo adicione link de vídeos.</t>
-  </si>
-  <si>
     <t>RN18</t>
   </si>
   <si>
@@ -269,9 +253,6 @@
     <t>O profissional autônomo pode gerar relatório de visualização de perfil e de serviços prestados.</t>
   </si>
   <si>
-    <t>O autônomo não-pagante pode cadastrar apenas uma profissão</t>
-  </si>
-  <si>
     <t>O sistema permite ao autônomo inserir fotos ilimitadamente de seus serviços.</t>
   </si>
   <si>
@@ -281,12 +262,6 @@
     <t>O contato feito pelo usuário do sistema deve ser respondido em até 2 dias, salvo em feriados e finais de semana.</t>
   </si>
   <si>
-    <t>O Autônomo pode fazer até 3 ofertas por dia em qualquer serviço proposto.</t>
-  </si>
-  <si>
-    <t>Autônomo Premium tem direito a fazer ilimitadas ofertas por dia em qualquer serviço proposto.</t>
-  </si>
-  <si>
     <t>RN24</t>
   </si>
   <si>
@@ -311,9 +286,6 @@
     <t>RN29</t>
   </si>
   <si>
-    <t>O cliente pode fechar o seu leilão.</t>
-  </si>
-  <si>
     <t>RN30</t>
   </si>
   <si>
@@ -329,40 +301,55 @@
     <t>RN33</t>
   </si>
   <si>
-    <t>RN34</t>
-  </si>
-  <si>
     <t>Os lances mais novos do leilão devem ser exibidos primeiro.</t>
   </si>
   <si>
-    <t>RN35</t>
-  </si>
-  <si>
     <t>Autonomo não pode fazer lances em areas de atuação que não sejam pertencentes a ele.</t>
   </si>
   <si>
+    <t>Para o cliente abrir um leilão, é necessário ser cadastrado no sistema.</t>
+  </si>
+  <si>
+    <t>O leilão poderá ficar aberto por até 30 dias.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O leilão deve conter data de abertura e de término, data de previsão, título e descrição do serviço. </t>
+  </si>
+  <si>
+    <t>O autônomo poderá fazer pesquisa de leilões.</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
     <t>Colunas1</t>
   </si>
   <si>
-    <t>O cliente pode abrir leilões ilimitadamente.</t>
-  </si>
-  <si>
-    <t>Para o cliente abrir um leilão, é necessário ser cadastrado no sistema.</t>
-  </si>
-  <si>
-    <t>O leilão poderá ficar aberto por até 30 dias.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">O leilão deve conter data de abertura e de término, data de previsão, título e descrição do serviço. </t>
-  </si>
-  <si>
-    <t>Um autonomo pode procurar novos leilões e visualizá-los.</t>
-  </si>
-  <si>
-    <t>O autônomo poderá fazer pesquisa de leilões.</t>
-  </si>
-  <si>
-    <t>O autônomo poderá ou não exibir suas informações de localização.</t>
+    <t>A pesquisa retornará 20 resultados por página</t>
+  </si>
+  <si>
+    <t>O autônomo não pagante não terá acesso ao leilão</t>
+  </si>
+  <si>
+    <t>O autônomo pagante do pacote de 30 dias terá direito a participar de 5 leilões</t>
+  </si>
+  <si>
+    <t>O autônomo pagante do pacote de 60 dias terá direito a participar de 20 leilões</t>
+  </si>
+  <si>
+    <t>O autônomo pagante do pacote de 30 dias terá acesso ilimitado ao leilão</t>
+  </si>
+  <si>
+    <t>O sistema permite que o autônomo adicione link de vídeos do youtube.</t>
+  </si>
+  <si>
+    <t>O cliente pode abrir uma quantidade ilimitada de leilões.</t>
+  </si>
+  <si>
+    <t>O cliente pode fechar seu leilão.</t>
+  </si>
+  <si>
+    <t>O leilão deverá ter uma duração mínima de 1 dia</t>
   </si>
 </sst>
 </file>
@@ -435,7 +422,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -449,6 +436,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -518,8 +506,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C37" totalsRowShown="0">
-  <autoFilter ref="A1:C37"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C34" totalsRowShown="0">
+  <autoFilter ref="A1:C34"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Código" dataDxfId="0"/>
     <tableColumn id="2" name="Descrição"/>
@@ -1026,16 +1014,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="101.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1046,7 +1033,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1078,261 +1065,242 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" t="s">
-        <v>84</v>
+        <v>66</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" t="s">
         <v>74</v>
-      </c>
-      <c r="B22" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B25" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B26" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="B27" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B31" t="s">
-        <v>109</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
         <v>97</v>
-      </c>
-      <c r="B32" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B33" t="s">
-        <v>111</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B34" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="B35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="B36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1342,16 +1310,4 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Nova regra de negócio
</commit_message>
<xml_diff>
--- a/EngenhariaSoftware/Regras de negócio v2.0.xlsx
+++ b/EngenhariaSoftware/Regras de negócio v2.0.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="111">
   <si>
     <t>Descrição</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>O leilão deverá ter uma duração mínima de 1 dia</t>
+  </si>
+  <si>
+    <t>RN34</t>
+  </si>
+  <si>
+    <t>O carrossel, da página principal, exibirá 3 perfis</t>
   </si>
 </sst>
 </file>
@@ -506,8 +512,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C34" totalsRowShown="0">
-  <autoFilter ref="A1:C34"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela2" displayName="Tabela2" ref="A1:C35" totalsRowShown="0">
+  <autoFilter ref="A1:C35"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Código" dataDxfId="0"/>
     <tableColumn id="2" name="Descrição"/>
@@ -1014,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,6 +1309,14 @@
         <v>93</v>
       </c>
     </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="B35" t="s">
+        <v>110</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>